<commit_message>
Fixed Splashscreen and replaced Score Background Texture with dynamic generated Texture
</commit_message>
<xml_diff>
--- a/ImagesSizes.xlsx
+++ b/ImagesSizes.xlsx
@@ -59,9 +59,6 @@
     <t>loadscreen</t>
   </si>
   <si>
-    <t>score_background</t>
-  </si>
-  <si>
     <t>btn_back</t>
   </si>
   <si>
@@ -252,6 +249,9 @@
   </si>
   <si>
     <t>108 x 2216</t>
+  </si>
+  <si>
+    <t>960 x 720</t>
   </si>
 </sst>
 </file>
@@ -331,8 +331,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="C40:H43" totalsRowShown="0">
-  <autoFilter ref="C40:H43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="C39:H42" totalsRowShown="0">
+  <autoFilter ref="C39:H42"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Handy"/>
     <tableColumn id="2" name="MDPI"/>
@@ -346,8 +346,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:M28" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A2:M28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:M27" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:M27"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Handy"/>
     <tableColumn id="2" name="Normal - mdpi"/>
@@ -630,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="115" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -656,7 +656,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -664,40 +664,40 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -705,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -721,7 +721,7 @@
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -729,7 +729,7 @@
         <v>5</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -737,7 +737,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -745,7 +745,7 @@
         <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -753,25 +753,31 @@
         <v>8</v>
       </c>
       <c r="L9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="L10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="L11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -779,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="L13" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -787,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -795,7 +801,7 @@
         <v>13</v>
       </c>
       <c r="L15" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -803,15 +809,15 @@
         <v>14</v>
       </c>
       <c r="L16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="L17" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -819,31 +825,31 @@
         <v>49</v>
       </c>
       <c r="L18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="L19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L20" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="L21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -851,7 +857,7 @@
         <v>17</v>
       </c>
       <c r="L22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -867,7 +873,7 @@
         <v>19</v>
       </c>
       <c r="L24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -883,43 +889,55 @@
         <v>21</v>
       </c>
       <c r="L26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="L27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>68</v>
-      </c>
-      <c r="L28" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F40" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G40" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H40" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.2">
@@ -927,24 +945,21 @@
         <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F41" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G41" t="s">
-        <v>37</v>
-      </c>
-      <c r="H41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -954,23 +969,6 @@
       </c>
       <c r="F42" t="s">
         <v>37</v>
-      </c>
-      <c r="G42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" t="s">
-        <v>36</v>
-      </c>
-      <c r="E43" t="s">
-        <v>37</v>
-      </c>
-      <c r="F43" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed List of Sprite Sizes
</commit_message>
<xml_diff>
--- a/ImagesSizes.xlsx
+++ b/ImagesSizes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25940" yWindow="8080" windowWidth="20900" windowHeight="22100" tabRatio="500"/>
+    <workbookView xWindow="17540" yWindow="4780" windowWidth="33500" windowHeight="22100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="180">
   <si>
     <t>Handy</t>
   </si>
@@ -194,45 +194,12 @@
     <t>460 x 460</t>
   </si>
   <si>
-    <t>220 x 220</t>
-  </si>
-  <si>
-    <t>895 x 190</t>
-  </si>
-  <si>
     <t>140 x 140</t>
   </si>
   <si>
-    <t>390 x 390</t>
-  </si>
-  <si>
-    <t>1020 x 1800</t>
-  </si>
-  <si>
-    <t>1000 x 850</t>
-  </si>
-  <si>
-    <t>880 x 150</t>
-  </si>
-  <si>
-    <t>400 x 116</t>
-  </si>
-  <si>
-    <t>910 x 250</t>
-  </si>
-  <si>
-    <t>715 x 215</t>
-  </si>
-  <si>
     <t>char</t>
   </si>
   <si>
-    <t>400 x 400</t>
-  </si>
-  <si>
-    <t>340 x 340</t>
-  </si>
-  <si>
     <t>1200 x ratio</t>
   </si>
   <si>
@@ -242,33 +209,18 @@
     <t>1080 x 1152</t>
   </si>
   <si>
-    <t>960 x 720</t>
-  </si>
-  <si>
-    <t>130 x 130</t>
-  </si>
-  <si>
-    <t>500 x 500</t>
-  </si>
-  <si>
     <t>348 x 172</t>
   </si>
   <si>
     <t>108 x 216</t>
   </si>
   <si>
-    <t>540 x 182</t>
-  </si>
-  <si>
     <t>720 x ratio</t>
   </si>
   <si>
     <t>720 x 768</t>
   </si>
   <si>
-    <t>90 x 90</t>
-  </si>
-  <si>
     <t>684 x 576</t>
   </si>
   <si>
@@ -278,24 +230,12 @@
     <t>662 x 140</t>
   </si>
   <si>
-    <t>576 x 433</t>
-  </si>
-  <si>
     <t>684 x 1216</t>
   </si>
   <si>
     <t>230 x 230</t>
   </si>
   <si>
-    <t>370 x 370</t>
-  </si>
-  <si>
-    <t>270 x 270</t>
-  </si>
-  <si>
-    <t>154 x 154</t>
-  </si>
-  <si>
     <t>396 x 133</t>
   </si>
   <si>
@@ -335,9 +275,6 @@
     <t>441 x 93</t>
   </si>
   <si>
-    <t>384 x 289</t>
-  </si>
-  <si>
     <t>456 x 811</t>
   </si>
   <si>
@@ -383,9 +320,6 @@
     <t>1026 x 864</t>
   </si>
   <si>
-    <t>996 x 212</t>
-  </si>
-  <si>
     <t>813 x 612</t>
   </si>
   <si>
@@ -471,13 +405,175 @@
   </si>
   <si>
     <t>144 x 288</t>
+  </si>
+  <si>
+    <t>320 x ratio</t>
+  </si>
+  <si>
+    <t>270 x 288</t>
+  </si>
+  <si>
+    <t>256 x 216</t>
+  </si>
+  <si>
+    <t>42 x 42</t>
+  </si>
+  <si>
+    <t>84 x 72</t>
+  </si>
+  <si>
+    <t>248 x 52</t>
+  </si>
+  <si>
+    <t>217 x 163</t>
+  </si>
+  <si>
+    <t>256 x 456</t>
+  </si>
+  <si>
+    <t>86 x 86</t>
+  </si>
+  <si>
+    <t>102 x 102</t>
+  </si>
+  <si>
+    <t>59 x 59</t>
+  </si>
+  <si>
+    <t>148 x 50</t>
+  </si>
+  <si>
+    <t>87 x 43</t>
+  </si>
+  <si>
+    <t>229 x 62</t>
+  </si>
+  <si>
+    <t>179 x 54</t>
+  </si>
+  <si>
+    <t>102 x 30</t>
+  </si>
+  <si>
+    <t>229 x 42</t>
+  </si>
+  <si>
+    <t>27 x 54</t>
+  </si>
+  <si>
+    <t>355 x 267</t>
+  </si>
+  <si>
+    <t>1600x 2560</t>
+  </si>
+  <si>
+    <t>542 x 408</t>
+  </si>
+  <si>
+    <t>600 x ratio</t>
+  </si>
+  <si>
+    <t>576 x 614</t>
+  </si>
+  <si>
+    <t>179 x 153</t>
+  </si>
+  <si>
+    <t>547 x 460</t>
+  </si>
+  <si>
+    <t>529 x 112</t>
+  </si>
+  <si>
+    <t>454 x 342</t>
+  </si>
+  <si>
+    <t>547 x 972</t>
+  </si>
+  <si>
+    <t>184 x 184</t>
+  </si>
+  <si>
+    <t>300 x 300</t>
+  </si>
+  <si>
+    <t>218 x 218</t>
+  </si>
+  <si>
+    <t>126 x 126</t>
+  </si>
+  <si>
+    <t>317 x 107</t>
+  </si>
+  <si>
+    <t>186 x 92</t>
+  </si>
+  <si>
+    <t>489 x 133</t>
+  </si>
+  <si>
+    <t>383 x 115</t>
+  </si>
+  <si>
+    <t>218 x 64</t>
+  </si>
+  <si>
+    <t>489 x 90</t>
+  </si>
+  <si>
+    <t>57 x 114</t>
+  </si>
+  <si>
+    <t>800 x ratio</t>
+  </si>
+  <si>
+    <t>100 x 100</t>
+  </si>
+  <si>
+    <t>158 x 158</t>
+  </si>
+  <si>
+    <t>374 x 374</t>
+  </si>
+  <si>
+    <t>273 x 273</t>
+  </si>
+  <si>
+    <t>565 x 425</t>
+  </si>
+  <si>
+    <t>1015 x 217</t>
+  </si>
+  <si>
+    <t>848 x 638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1600 x 2560 </t>
+  </si>
+  <si>
+    <t>1600 x ratio</t>
+  </si>
+  <si>
+    <t>1132 x 852</t>
+  </si>
+  <si>
+    <t>577 x 434</t>
+  </si>
+  <si>
+    <t>865 x 651</t>
+  </si>
+  <si>
+    <t>1600 x -1</t>
+  </si>
+  <si>
+    <t>1154 x 869</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -505,6 +601,22 @@
       <color theme="1"/>
       <name val="Calibri (Textkörper)"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -514,7 +626,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -522,21 +634,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -593,7 +791,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:M27" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:M27" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A2:M27"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Handy"/>
@@ -602,12 +800,12 @@
     <tableColumn id="4" name="Normal - xhdpi"/>
     <tableColumn id="5" name="Normal - xxhdpi"/>
     <tableColumn id="6" name="Normal - xxxhdpi"/>
-    <tableColumn id="7" name="Large - mdpi"/>
+    <tableColumn id="7" name="Large - mdpi" dataDxfId="1"/>
     <tableColumn id="8" name="Large - hdpi"/>
     <tableColumn id="9" name="Large - xhdpi"/>
-    <tableColumn id="10" name="Large - xxhdpi"/>
+    <tableColumn id="10" name="Large - xxhdpi" dataDxfId="0"/>
     <tableColumn id="11" name="X-Large - mdpi"/>
-    <tableColumn id="12" name="X-Large - hdpi" dataDxfId="0"/>
+    <tableColumn id="12" name="X-Large - hdpi" dataDxfId="2"/>
     <tableColumn id="13" name="X-Large - xhdpi"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -880,7 +1078,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -925,7 +1123,7 @@
       <c r="F2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -934,7 +1132,7 @@
       <c r="I2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="9" t="s">
         <v>50</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -951,26 +1149,50 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>130</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>68</v>
+        <v>108</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="K3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
       <c r="C4" t="s">
         <v>29</v>
       </c>
@@ -978,476 +1200,977 @@
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="G4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
         <v>36</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
       </c>
       <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="K5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F6" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" t="s">
-        <v>131</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>132</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F7" t="s">
-        <v>133</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>60</v>
+      <c r="D7" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>134</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>69</v>
+        <v>111</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>171</v>
       </c>
       <c r="F9" t="s">
-        <v>135</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>56</v>
+        <v>113</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" t="s">
+        <v>171</v>
+      </c>
+      <c r="J9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="M9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>71</v>
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>59</v>
+        <v>115</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F12" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>67</v>
+      <c r="G12" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" t="s">
+        <v>99</v>
+      </c>
+      <c r="M12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
       <c r="C13" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>73</v>
+        <v>116</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H13" t="s">
+        <v>168</v>
+      </c>
+      <c r="I13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" t="s">
+        <v>168</v>
+      </c>
+      <c r="L13" t="s">
+        <v>100</v>
+      </c>
+      <c r="M13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>135</v>
+      </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="F14" t="s">
-        <v>139</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>58</v>
+        <v>117</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14" t="s">
+        <v>169</v>
+      </c>
+      <c r="I14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J14" t="s">
+        <v>117</v>
+      </c>
+      <c r="K14" t="s">
+        <v>169</v>
+      </c>
+      <c r="L14" t="s">
+        <v>101</v>
+      </c>
+      <c r="M14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="F15" t="s">
-        <v>139</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>66</v>
+        <v>117</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="H15" t="s">
+        <v>169</v>
+      </c>
+      <c r="I15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J15" t="s">
+        <v>117</v>
+      </c>
+      <c r="K15" t="s">
+        <v>169</v>
+      </c>
+      <c r="L15" t="s">
+        <v>101</v>
+      </c>
+      <c r="M15" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="F16" t="s">
-        <v>139</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16" t="s">
+        <v>169</v>
+      </c>
+      <c r="I16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J16" t="s">
+        <v>117</v>
+      </c>
+      <c r="K16" t="s">
+        <v>169</v>
+      </c>
+      <c r="L16" t="s">
+        <v>101</v>
+      </c>
+      <c r="M16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
       <c r="C17" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" t="s">
+        <v>167</v>
+      </c>
+      <c r="I17" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" t="s">
+        <v>118</v>
+      </c>
+      <c r="K17" t="s">
+        <v>167</v>
+      </c>
+      <c r="L17" t="s">
+        <v>102</v>
+      </c>
+      <c r="M17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>49</v>
       </c>
+      <c r="B18" t="s">
+        <v>136</v>
+      </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>167</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>140</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H18" t="s">
+        <v>167</v>
+      </c>
+      <c r="I18" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" t="s">
+        <v>118</v>
+      </c>
+      <c r="K18" t="s">
+        <v>167</v>
+      </c>
+      <c r="L18" t="s">
+        <v>102</v>
+      </c>
+      <c r="M18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
+      <c r="B19" t="s">
+        <v>136</v>
+      </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>140</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H19" t="s">
+        <v>167</v>
+      </c>
+      <c r="I19" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" t="s">
+        <v>118</v>
+      </c>
+      <c r="K19" t="s">
+        <v>167</v>
+      </c>
+      <c r="L19" t="s">
+        <v>102</v>
+      </c>
+      <c r="M19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
+      <c r="B20" t="s">
+        <v>137</v>
+      </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" t="s">
+        <v>119</v>
+      </c>
+      <c r="K20" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" t="s">
+        <v>103</v>
+      </c>
+      <c r="M20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
+      <c r="B21" t="s">
+        <v>138</v>
+      </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>142</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H21" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" t="s">
+        <v>120</v>
+      </c>
+      <c r="K21" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" t="s">
+        <v>60</v>
+      </c>
+      <c r="M21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
+      <c r="B22" t="s">
+        <v>139</v>
+      </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H22" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" t="s">
+        <v>121</v>
+      </c>
+      <c r="K22" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" t="s">
+        <v>104</v>
+      </c>
+      <c r="M22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>18</v>
       </c>
+      <c r="B23" t="s">
+        <v>140</v>
+      </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H23" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J23" t="s">
+        <v>122</v>
+      </c>
+      <c r="K23" t="s">
+        <v>72</v>
+      </c>
+      <c r="L23" t="s">
+        <v>105</v>
+      </c>
+      <c r="M23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>142</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H24" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" t="s">
+        <v>60</v>
+      </c>
+      <c r="J24" t="s">
+        <v>120</v>
+      </c>
+      <c r="K24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" t="s">
+        <v>60</v>
+      </c>
+      <c r="M24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>20</v>
       </c>
+      <c r="B25" t="s">
+        <v>141</v>
+      </c>
       <c r="C25" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="F25" t="s">
-        <v>145</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" t="s">
+        <v>123</v>
+      </c>
+      <c r="K25" t="s">
+        <v>73</v>
+      </c>
+      <c r="L25" t="s">
+        <v>106</v>
+      </c>
+      <c r="M25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
+      <c r="B26" t="s">
+        <v>142</v>
+      </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="F26" t="s">
-        <v>146</v>
-      </c>
-      <c r="L26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" t="s">
+        <v>107</v>
+      </c>
+      <c r="J26" t="s">
+        <v>124</v>
+      </c>
+      <c r="K26" t="s">
+        <v>74</v>
+      </c>
+      <c r="L26" t="s">
+        <v>107</v>
+      </c>
+      <c r="M26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H27" t="s">
         <v>75</v>
       </c>
-      <c r="F27" t="s">
-        <v>147</v>
-      </c>
-      <c r="L27" s="2" t="s">
+      <c r="I27" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" t="s">
+        <v>125</v>
+      </c>
+      <c r="K27" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>61</v>
+      </c>
+      <c r="M27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +2190,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -1481,7 +2204,7 @@
         <v>33</v>
       </c>
       <c r="F32" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="G32" t="s">
         <v>38</v>
@@ -1501,7 +2224,7 @@
         <v>36</v>
       </c>
       <c r="F33" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
@@ -1520,6 +2243,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Exported images to res folder
</commit_message>
<xml_diff>
--- a/ImagesSizes.xlsx
+++ b/ImagesSizes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17540" yWindow="4780" windowWidth="33500" windowHeight="22100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -573,7 +573,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -617,6 +617,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -626,27 +633,9 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -657,9 +646,7 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -681,48 +668,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -747,6 +732,30 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -791,7 +800,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:M27" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:M27" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A2:M27"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Handy"/>
@@ -800,12 +809,12 @@
     <tableColumn id="4" name="Normal - xhdpi"/>
     <tableColumn id="5" name="Normal - xxhdpi"/>
     <tableColumn id="6" name="Normal - xxxhdpi"/>
-    <tableColumn id="7" name="Large - mdpi" dataDxfId="1"/>
+    <tableColumn id="7" name="Large - mdpi" dataDxfId="3"/>
     <tableColumn id="8" name="Large - hdpi"/>
     <tableColumn id="9" name="Large - xhdpi"/>
-    <tableColumn id="10" name="Large - xxhdpi" dataDxfId="0"/>
-    <tableColumn id="11" name="X-Large - mdpi"/>
-    <tableColumn id="12" name="X-Large - hdpi" dataDxfId="2"/>
+    <tableColumn id="10" name="Large - xxhdpi" dataDxfId="2"/>
+    <tableColumn id="11" name="X-Large - mdpi" dataDxfId="0"/>
+    <tableColumn id="12" name="X-Large - hdpi" dataDxfId="1"/>
     <tableColumn id="13" name="X-Large - xhdpi"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1078,7 +1087,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1123,7 +1132,7 @@
       <c r="F2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1132,7 +1141,7 @@
       <c r="I2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="6" t="s">
         <v>50</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -1164,7 +1173,7 @@
       <c r="F3" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>147</v>
       </c>
       <c r="H3" t="s">
@@ -1173,13 +1182,13 @@
       <c r="I3" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>57</v>
       </c>
       <c r="M3" t="s">
@@ -1190,163 +1199,163 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G6" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J6" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L6" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M6" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="7" t="s">
         <v>110</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="7" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1354,22 +1363,22 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="10" t="s">
         <v>150</v>
       </c>
       <c r="H8" t="s">
@@ -1381,10 +1390,10 @@
       <c r="J8" t="s">
         <v>111</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>96</v>
       </c>
       <c r="M8" t="s">
@@ -1395,22 +1404,22 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="10" t="s">
         <v>151</v>
       </c>
       <c r="H9" t="s">
@@ -1422,10 +1431,10 @@
       <c r="J9" t="s">
         <v>113</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>171</v>
       </c>
       <c r="M9" t="s">
@@ -1436,22 +1445,22 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="10" t="s">
         <v>148</v>
       </c>
       <c r="H10" t="s">
@@ -1463,7 +1472,7 @@
       <c r="J10" t="s">
         <v>109</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="5" t="s">
         <v>63</v>
       </c>
       <c r="L10" t="s">
@@ -1477,22 +1486,22 @@
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="10" t="s">
         <v>153</v>
       </c>
       <c r="H11" t="s">
@@ -1504,7 +1513,7 @@
       <c r="J11" t="s">
         <v>115</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="5" t="s">
         <v>67</v>
       </c>
       <c r="L11" t="s">
@@ -1518,22 +1527,22 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="10" t="s">
         <v>154</v>
       </c>
       <c r="H12" t="s">
@@ -1545,7 +1554,7 @@
       <c r="J12" t="s">
         <v>54</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="5" t="s">
         <v>68</v>
       </c>
       <c r="L12" t="s">
@@ -1559,22 +1568,22 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="10" t="s">
         <v>155</v>
       </c>
       <c r="H13" t="s">
@@ -1586,7 +1595,7 @@
       <c r="J13" t="s">
         <v>116</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="5" t="s">
         <v>168</v>
       </c>
       <c r="L13" t="s">
@@ -1600,22 +1609,22 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="10" t="s">
         <v>156</v>
       </c>
       <c r="H14" t="s">
@@ -1627,7 +1636,7 @@
       <c r="J14" t="s">
         <v>117</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="5" t="s">
         <v>169</v>
       </c>
       <c r="L14" t="s">
@@ -1641,22 +1650,22 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="10" t="s">
         <v>156</v>
       </c>
       <c r="H15" t="s">
@@ -1668,7 +1677,7 @@
       <c r="J15" t="s">
         <v>117</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="5" t="s">
         <v>169</v>
       </c>
       <c r="L15" t="s">
@@ -1682,22 +1691,22 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="10" t="s">
         <v>156</v>
       </c>
       <c r="H16" t="s">
@@ -1709,7 +1718,7 @@
       <c r="J16" t="s">
         <v>117</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="5" t="s">
         <v>169</v>
       </c>
       <c r="L16" t="s">
@@ -1723,22 +1732,22 @@
       <c r="A17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="10" t="s">
         <v>157</v>
       </c>
       <c r="H17" t="s">
@@ -1750,7 +1759,7 @@
       <c r="J17" t="s">
         <v>118</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="5" t="s">
         <v>167</v>
       </c>
       <c r="L17" t="s">
@@ -1764,22 +1773,22 @@
       <c r="A18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="10" t="s">
         <v>157</v>
       </c>
       <c r="H18" t="s">
@@ -1791,7 +1800,7 @@
       <c r="J18" t="s">
         <v>118</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="5" t="s">
         <v>167</v>
       </c>
       <c r="L18" t="s">
@@ -1805,22 +1814,22 @@
       <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="10" t="s">
         <v>157</v>
       </c>
       <c r="H19" t="s">
@@ -1832,7 +1841,7 @@
       <c r="J19" t="s">
         <v>118</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="5" t="s">
         <v>167</v>
       </c>
       <c r="L19" t="s">
@@ -1846,22 +1855,22 @@
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="10" t="s">
         <v>158</v>
       </c>
       <c r="H20" t="s">
@@ -1873,7 +1882,7 @@
       <c r="J20" t="s">
         <v>119</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="5" t="s">
         <v>69</v>
       </c>
       <c r="L20" t="s">
@@ -1887,22 +1896,22 @@
       <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="10" t="s">
         <v>159</v>
       </c>
       <c r="H21" t="s">
@@ -1914,7 +1923,7 @@
       <c r="J21" t="s">
         <v>120</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="5" t="s">
         <v>70</v>
       </c>
       <c r="L21" t="s">
@@ -1928,22 +1937,22 @@
       <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="10" t="s">
         <v>160</v>
       </c>
       <c r="H22" t="s">
@@ -1955,7 +1964,7 @@
       <c r="J22" t="s">
         <v>121</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="5" t="s">
         <v>71</v>
       </c>
       <c r="L22" t="s">
@@ -1969,22 +1978,22 @@
       <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="10" t="s">
         <v>161</v>
       </c>
       <c r="H23" t="s">
@@ -1996,7 +2005,7 @@
       <c r="J23" t="s">
         <v>122</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="5" t="s">
         <v>72</v>
       </c>
       <c r="L23" t="s">
@@ -2010,22 +2019,22 @@
       <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="10" t="s">
         <v>159</v>
       </c>
       <c r="H24" t="s">
@@ -2037,7 +2046,7 @@
       <c r="J24" t="s">
         <v>120</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="5" t="s">
         <v>70</v>
       </c>
       <c r="L24" t="s">
@@ -2051,22 +2060,22 @@
       <c r="A25" t="s">
         <v>20</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="10" t="s">
         <v>162</v>
       </c>
       <c r="H25" t="s">
@@ -2078,7 +2087,7 @@
       <c r="J25" t="s">
         <v>123</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="5" t="s">
         <v>73</v>
       </c>
       <c r="L25" t="s">
@@ -2092,22 +2101,22 @@
       <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="10" t="s">
         <v>163</v>
       </c>
       <c r="H26" t="s">
@@ -2119,7 +2128,7 @@
       <c r="J26" t="s">
         <v>124</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="5" t="s">
         <v>74</v>
       </c>
       <c r="L26" t="s">
@@ -2133,22 +2142,22 @@
       <c r="A27" t="s">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="10" t="s">
         <v>164</v>
       </c>
       <c r="H27" t="s">
@@ -2160,7 +2169,7 @@
       <c r="J27" t="s">
         <v>125</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="5" t="s">
         <v>75</v>
       </c>
       <c r="L27" t="s">

</xml_diff>

<commit_message>
Fixed bugs and changed background on Normal
</commit_message>
<xml_diff>
--- a/ImagesSizes.xlsx
+++ b/ImagesSizes.xlsx
@@ -685,7 +685,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -699,7 +699,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -708,18 +707,6 @@
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -732,6 +719,18 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -813,8 +812,8 @@
     <tableColumn id="8" name="Large - hdpi"/>
     <tableColumn id="9" name="Large - xhdpi"/>
     <tableColumn id="10" name="Large - xxhdpi" dataDxfId="2"/>
-    <tableColumn id="11" name="X-Large - mdpi" dataDxfId="0"/>
-    <tableColumn id="12" name="X-Large - hdpi" dataDxfId="1"/>
+    <tableColumn id="11" name="X-Large - mdpi" dataDxfId="1"/>
+    <tableColumn id="12" name="X-Large - hdpi" dataDxfId="0"/>
     <tableColumn id="13" name="X-Large - xhdpi"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1087,7 +1086,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,7 +1222,7 @@
       <c r="I4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="13" t="s">
         <v>173</v>
       </c>
       <c r="K4" s="10" t="s">
@@ -1281,34 +1280,34 @@
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>112</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="13" t="s">
         <v>58</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="10" t="s">
         <v>65</v>
       </c>
       <c r="L6" s="13" t="s">
@@ -1322,34 +1321,34 @@
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>110</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="13" t="s">
         <v>55</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="10" t="s">
         <v>166</v>
       </c>
       <c r="L7" s="13" t="s">
@@ -1381,19 +1380,19 @@
       <c r="G8" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="9" t="s">
         <v>96</v>
       </c>
       <c r="J8" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="9" t="s">
         <v>96</v>
       </c>
       <c r="M8" t="s">
@@ -1422,19 +1421,19 @@
       <c r="G9" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="9" t="s">
         <v>171</v>
       </c>
       <c r="J9" t="s">
         <v>113</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="9" t="s">
         <v>171</v>
       </c>
       <c r="M9" t="s">
@@ -1463,19 +1462,19 @@
       <c r="G10" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="9" t="s">
         <v>59</v>
       </c>
       <c r="J10" t="s">
         <v>109</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="9" t="s">
         <v>59</v>
       </c>
       <c r="M10" t="s">
@@ -1504,19 +1503,19 @@
       <c r="G11" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="9" t="s">
         <v>98</v>
       </c>
       <c r="J11" t="s">
         <v>115</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="9" t="s">
         <v>98</v>
       </c>
       <c r="M11" t="s">
@@ -1545,19 +1544,19 @@
       <c r="G12" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="9" t="s">
         <v>99</v>
       </c>
       <c r="J12" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="9" t="s">
         <v>99</v>
       </c>
       <c r="M12" t="s">
@@ -1586,19 +1585,19 @@
       <c r="G13" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="9" t="s">
         <v>100</v>
       </c>
       <c r="J13" t="s">
         <v>116</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="9" t="s">
         <v>100</v>
       </c>
       <c r="M13" t="s">
@@ -1627,19 +1626,19 @@
       <c r="G14" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="9" t="s">
         <v>101</v>
       </c>
       <c r="J14" t="s">
         <v>117</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="9" t="s">
         <v>101</v>
       </c>
       <c r="M14" t="s">
@@ -1668,19 +1667,19 @@
       <c r="G15" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="9" t="s">
         <v>101</v>
       </c>
       <c r="J15" t="s">
         <v>117</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="9" t="s">
         <v>101</v>
       </c>
       <c r="M15" t="s">
@@ -1709,19 +1708,19 @@
       <c r="G16" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="9" t="s">
         <v>101</v>
       </c>
       <c r="J16" t="s">
         <v>117</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="9" t="s">
         <v>101</v>
       </c>
       <c r="M16" t="s">
@@ -1750,19 +1749,19 @@
       <c r="G17" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="9" t="s">
         <v>102</v>
       </c>
       <c r="J17" t="s">
         <v>118</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="9" t="s">
         <v>102</v>
       </c>
       <c r="M17" t="s">
@@ -1791,19 +1790,19 @@
       <c r="G18" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="9" t="s">
         <v>102</v>
       </c>
       <c r="J18" t="s">
         <v>118</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="9" t="s">
         <v>102</v>
       </c>
       <c r="M18" t="s">
@@ -1832,19 +1831,19 @@
       <c r="G19" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="9" t="s">
         <v>102</v>
       </c>
       <c r="J19" t="s">
         <v>118</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="9" t="s">
         <v>102</v>
       </c>
       <c r="M19" t="s">
@@ -1873,19 +1872,19 @@
       <c r="G20" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="9" t="s">
         <v>103</v>
       </c>
       <c r="J20" t="s">
         <v>119</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="9" t="s">
         <v>103</v>
       </c>
       <c r="M20" t="s">
@@ -1914,19 +1913,19 @@
       <c r="G21" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="9" t="s">
         <v>60</v>
       </c>
       <c r="J21" t="s">
         <v>120</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="9" t="s">
         <v>60</v>
       </c>
       <c r="M21" t="s">
@@ -1955,19 +1954,19 @@
       <c r="G22" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="9" t="s">
         <v>104</v>
       </c>
       <c r="J22" t="s">
         <v>121</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K22" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="9" t="s">
         <v>104</v>
       </c>
       <c r="M22" t="s">
@@ -1996,19 +1995,19 @@
       <c r="G23" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="9" t="s">
         <v>105</v>
       </c>
       <c r="J23" t="s">
         <v>122</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="9" t="s">
         <v>105</v>
       </c>
       <c r="M23" t="s">
@@ -2037,19 +2036,19 @@
       <c r="G24" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="9" t="s">
         <v>60</v>
       </c>
       <c r="J24" t="s">
         <v>120</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K24" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="9" t="s">
         <v>60</v>
       </c>
       <c r="M24" t="s">
@@ -2078,19 +2077,19 @@
       <c r="G25" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="9" t="s">
         <v>106</v>
       </c>
       <c r="J25" t="s">
         <v>123</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="9" t="s">
         <v>106</v>
       </c>
       <c r="M25" t="s">
@@ -2119,19 +2118,19 @@
       <c r="G26" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="9" t="s">
         <v>107</v>
       </c>
       <c r="J26" t="s">
         <v>124</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K26" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="9" t="s">
         <v>107</v>
       </c>
       <c r="M26" t="s">
@@ -2160,19 +2159,19 @@
       <c r="G27" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="9" t="s">
         <v>61</v>
       </c>
       <c r="J27" t="s">
         <v>125</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="K27" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="9" t="s">
         <v>61</v>
       </c>
       <c r="M27" t="s">

</xml_diff>

<commit_message>
Background and Cliff rework
</commit_message>
<xml_diff>
--- a/ImagesSizes.xlsx
+++ b/ImagesSizes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -597,11 +597,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Textkörper)"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -623,6 +618,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri (Textkörper)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -682,10 +682,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -695,11 +695,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -1086,7 +1089,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="115" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1160,16 +1163,16 @@
       <c r="B3" t="s">
         <v>126</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="9" t="s">
         <v>108</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -1198,7 +1201,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1213,25 +1216,25 @@
       <c r="F4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1239,40 +1242,40 @@
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="13" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1280,40 +1283,40 @@
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>112</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="11" t="s">
         <v>112</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="11" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1321,40 +1324,40 @@
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="11" t="s">
         <v>110</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="11" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1386,7 +1389,7 @@
       <c r="I8" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="9" t="s">
         <v>111</v>
       </c>
       <c r="K8" s="10" t="s">
@@ -1395,7 +1398,7 @@
       <c r="L8" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="9" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1427,7 +1430,7 @@
       <c r="I9" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="9" t="s">
         <v>113</v>
       </c>
       <c r="K9" s="10" t="s">
@@ -1436,7 +1439,7 @@
       <c r="L9" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="9" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1468,7 +1471,7 @@
       <c r="I10" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="9" t="s">
         <v>109</v>
       </c>
       <c r="K10" s="10" t="s">
@@ -1477,7 +1480,7 @@
       <c r="L10" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1509,7 +1512,7 @@
       <c r="I11" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="9" t="s">
         <v>115</v>
       </c>
       <c r="K11" s="10" t="s">
@@ -1518,7 +1521,7 @@
       <c r="L11" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="9" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1550,7 +1553,7 @@
       <c r="I12" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="9" t="s">
         <v>54</v>
       </c>
       <c r="K12" s="10" t="s">
@@ -1559,7 +1562,7 @@
       <c r="L12" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="9" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1591,7 +1594,7 @@
       <c r="I13" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="9" t="s">
         <v>116</v>
       </c>
       <c r="K13" s="10" t="s">
@@ -1600,7 +1603,7 @@
       <c r="L13" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="9" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1632,7 +1635,7 @@
       <c r="I14" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="9" t="s">
         <v>117</v>
       </c>
       <c r="K14" s="10" t="s">
@@ -1641,7 +1644,7 @@
       <c r="L14" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="9" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1673,7 +1676,7 @@
       <c r="I15" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="9" t="s">
         <v>117</v>
       </c>
       <c r="K15" s="10" t="s">
@@ -1682,7 +1685,7 @@
       <c r="L15" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="9" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1714,7 +1717,7 @@
       <c r="I16" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="9" t="s">
         <v>117</v>
       </c>
       <c r="K16" s="10" t="s">
@@ -1723,7 +1726,7 @@
       <c r="L16" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="9" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1755,7 +1758,7 @@
       <c r="I17" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="9" t="s">
         <v>118</v>
       </c>
       <c r="K17" s="10" t="s">
@@ -1764,7 +1767,7 @@
       <c r="L17" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="9" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1796,7 +1799,7 @@
       <c r="I18" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="9" t="s">
         <v>118</v>
       </c>
       <c r="K18" s="10" t="s">
@@ -1805,7 +1808,7 @@
       <c r="L18" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="9" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1837,7 +1840,7 @@
       <c r="I19" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="9" t="s">
         <v>118</v>
       </c>
       <c r="K19" s="10" t="s">
@@ -1846,7 +1849,7 @@
       <c r="L19" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="9" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1878,7 +1881,7 @@
       <c r="I20" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="9" t="s">
         <v>119</v>
       </c>
       <c r="K20" s="10" t="s">
@@ -1887,7 +1890,7 @@
       <c r="L20" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="9" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1919,7 +1922,7 @@
       <c r="I21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="9" t="s">
         <v>120</v>
       </c>
       <c r="K21" s="10" t="s">
@@ -1928,7 +1931,7 @@
       <c r="L21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="9" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1960,7 +1963,7 @@
       <c r="I22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="9" t="s">
         <v>121</v>
       </c>
       <c r="K22" s="10" t="s">
@@ -1969,7 +1972,7 @@
       <c r="L22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="9" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2001,7 +2004,7 @@
       <c r="I23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="9" t="s">
         <v>122</v>
       </c>
       <c r="K23" s="10" t="s">
@@ -2010,7 +2013,7 @@
       <c r="L23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="9" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2042,7 +2045,7 @@
       <c r="I24" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="9" t="s">
         <v>120</v>
       </c>
       <c r="K24" s="10" t="s">
@@ -2051,7 +2054,7 @@
       <c r="L24" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="9" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2083,7 +2086,7 @@
       <c r="I25" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="9" t="s">
         <v>123</v>
       </c>
       <c r="K25" s="10" t="s">
@@ -2092,7 +2095,7 @@
       <c r="L25" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="9" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2124,7 +2127,7 @@
       <c r="I26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="9" t="s">
         <v>124</v>
       </c>
       <c r="K26" s="10" t="s">
@@ -2133,7 +2136,7 @@
       <c r="L26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="9" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2165,7 +2168,7 @@
       <c r="I27" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="9" t="s">
         <v>125</v>
       </c>
       <c r="K27" s="10" t="s">
@@ -2174,7 +2177,7 @@
       <c r="L27" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="9" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>